<commit_message>
Fixed combined analysis function
</commit_message>
<xml_diff>
--- a/exports/lsmean_files/HIF 5 - LSMeans.xlsx
+++ b/exports/lsmean_files/HIF 5 - LSMeans.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">Genotype</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t xml:space="preserve">Seed weight (grams)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sq</t>
   </si>
   <si>
     <t xml:space="preserve">Test weight</t>
@@ -505,13 +508,14 @@
     <col min="6" max="6" width="19.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="13.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="19.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="11.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="13.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="5.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="11.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="13.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2">
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -521,6 +525,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -553,10 +558,13 @@
       <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K3" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>23</v>
@@ -580,15 +588,18 @@
         <v>12.3</v>
       </c>
       <c r="I4" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>56.5</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="K4" s="1" t="n">
         <v>1902.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>27.5</v>
@@ -612,15 +623,18 @@
         <v>11.8</v>
       </c>
       <c r="I5" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <v>57.6</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="K5" s="1" t="n">
         <v>2247.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45</v>
@@ -644,15 +658,18 @@
         <v>16.1</v>
       </c>
       <c r="I6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>56.2</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="K6" s="1" t="n">
         <v>1606.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>45.5</v>
@@ -676,15 +693,18 @@
         <v>15</v>
       </c>
       <c r="I7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="n">
         <v>57.5</v>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="K7" s="1" t="n">
         <v>1201.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>44.5</v>
@@ -708,15 +728,18 @@
         <v>15</v>
       </c>
       <c r="I8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="n">
         <v>56.7</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="K8" s="1" t="n">
         <v>1393.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>28.5</v>
@@ -740,15 +763,18 @@
         <v>13.4</v>
       </c>
       <c r="I9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1" t="n">
         <v>57.5</v>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="K9" s="1" t="n">
         <v>1823.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>22.5</v>
@@ -772,15 +798,18 @@
         <v>12.9</v>
       </c>
       <c r="I10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="J10" s="1" t="n">
+      <c r="K10" s="1" t="n">
         <v>2204.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>24.5</v>
@@ -804,15 +833,18 @@
         <v>13.2</v>
       </c>
       <c r="I11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1" t="n">
         <v>57.6</v>
       </c>
-      <c r="J11" s="1" t="n">
+      <c r="K11" s="1" t="n">
         <v>2100.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>24</v>
@@ -836,15 +868,18 @@
         <v>12.8</v>
       </c>
       <c r="I12" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J12" s="1" t="n">
         <v>58.3</v>
       </c>
-      <c r="J12" s="1" t="n">
+      <c r="K12" s="1" t="n">
         <v>2202.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>23</v>
@@ -868,15 +903,18 @@
         <v>13.1</v>
       </c>
       <c r="I13" s="1" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J13" s="1" t="n">
         <v>57.6</v>
       </c>
-      <c r="J13" s="1" t="n">
+      <c r="K13" s="1" t="n">
         <v>1832.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>22</v>
@@ -900,15 +938,18 @@
         <v>12.7</v>
       </c>
       <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1" t="n">
         <v>57.5</v>
       </c>
-      <c r="J14" s="1" t="n">
+      <c r="K14" s="1" t="n">
         <v>1793.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>20.5</v>
@@ -932,15 +973,18 @@
         <v>13.8</v>
       </c>
       <c r="I15" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J15" s="1" t="n">
         <v>57.3</v>
       </c>
-      <c r="J15" s="1" t="n">
+      <c r="K15" s="1" t="n">
         <v>2006.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>24.5</v>
@@ -964,15 +1008,18 @@
         <v>13.8</v>
       </c>
       <c r="I16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J16" s="1" t="n">
         <v>57.6</v>
       </c>
-      <c r="J16" s="1" t="n">
+      <c r="K16" s="1" t="n">
         <v>1998.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>22</v>
@@ -996,15 +1043,18 @@
         <v>14.5</v>
       </c>
       <c r="I17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1" t="n">
         <v>57.8</v>
       </c>
-      <c r="J17" s="1" t="n">
+      <c r="K17" s="1" t="n">
         <v>2103</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>28.5</v>
@@ -1028,15 +1078,18 @@
         <v>15.8</v>
       </c>
       <c r="I18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1" t="n">
         <v>57.5</v>
       </c>
-      <c r="J18" s="1" t="n">
+      <c r="K18" s="1" t="n">
         <v>2156.3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>24</v>
@@ -1060,15 +1113,18 @@
         <v>15.5</v>
       </c>
       <c r="I19" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J19" s="1" t="n">
         <v>58.2</v>
       </c>
-      <c r="J19" s="1" t="n">
+      <c r="K19" s="1" t="n">
         <v>1891.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>24.5</v>
@@ -1092,15 +1148,18 @@
         <v>14.5</v>
       </c>
       <c r="I20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1" t="n">
         <v>58.7</v>
       </c>
-      <c r="J20" s="1" t="n">
+      <c r="K20" s="1" t="n">
         <v>2100</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>29</v>
@@ -1124,15 +1183,18 @@
         <v>16.6</v>
       </c>
       <c r="I21" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J21" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="J21" s="1" t="n">
+      <c r="K21" s="1" t="n">
         <v>1862.8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>27</v>
@@ -1156,15 +1218,18 @@
         <v>16.1</v>
       </c>
       <c r="I22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1" t="n">
         <v>56.6</v>
       </c>
-      <c r="J22" s="1" t="n">
+      <c r="K22" s="1" t="n">
         <v>1861.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>26</v>
@@ -1188,15 +1253,18 @@
         <v>14.6</v>
       </c>
       <c r="I23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" s="1" t="n">
         <v>57.6</v>
       </c>
-      <c r="J23" s="1" t="n">
+      <c r="K23" s="1" t="n">
         <v>1963.3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>32.5</v>
@@ -1220,15 +1288,18 @@
         <v>14.4</v>
       </c>
       <c r="I24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1" t="n">
         <v>57.8</v>
       </c>
-      <c r="J24" s="1" t="n">
+      <c r="K24" s="1" t="n">
         <v>1882.1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>27</v>
@@ -1252,15 +1323,18 @@
         <v>14.1</v>
       </c>
       <c r="I25" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J25" s="1" t="n">
         <v>57.2</v>
       </c>
-      <c r="J25" s="1" t="n">
+      <c r="K25" s="1" t="n">
         <v>1930.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>28</v>
@@ -1284,15 +1358,18 @@
         <v>16.3</v>
       </c>
       <c r="I26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J26" s="1" t="n">
         <v>56.5</v>
       </c>
-      <c r="J26" s="1" t="n">
+      <c r="K26" s="1" t="n">
         <v>2041.8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>20.5</v>
@@ -1316,15 +1393,18 @@
         <v>13.5</v>
       </c>
       <c r="I27" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J27" s="1" t="n">
         <v>57.7</v>
       </c>
-      <c r="J27" s="1" t="n">
+      <c r="K27" s="1" t="n">
         <v>2265.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>49</v>
@@ -1348,15 +1428,18 @@
         <v>12.4</v>
       </c>
       <c r="I28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J28" s="1" t="n">
         <v>57.9</v>
       </c>
-      <c r="J28" s="1" t="n">
+      <c r="K28" s="1" t="n">
         <v>1379.9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>51.5</v>
@@ -1380,15 +1463,18 @@
         <v>14.1</v>
       </c>
       <c r="I29" s="1" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J29" s="1" t="n">
         <v>57.1</v>
       </c>
-      <c r="J29" s="1" t="n">
+      <c r="K29" s="1" t="n">
         <v>1254.2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>48.5</v>
@@ -1412,15 +1498,18 @@
         <v>13.8</v>
       </c>
       <c r="I30" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J30" s="1" t="n">
         <v>57.2</v>
       </c>
-      <c r="J30" s="1" t="n">
+      <c r="K30" s="1" t="n">
         <v>1324.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>53</v>
@@ -1444,15 +1533,18 @@
         <v>11.8</v>
       </c>
       <c r="I31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J31" s="1" t="n">
         <v>57.2</v>
       </c>
-      <c r="J31" s="1" t="n">
+      <c r="K31" s="1" t="n">
         <v>1387.2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>45.5</v>
@@ -1476,15 +1568,18 @@
         <v>12.3</v>
       </c>
       <c r="I32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1" t="n">
         <v>57.9</v>
       </c>
-      <c r="J32" s="1" t="n">
+      <c r="K32" s="1" t="n">
         <v>1364.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>34</v>
@@ -1508,15 +1603,18 @@
         <v>14.5</v>
       </c>
       <c r="I33" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J33" s="1" t="n">
         <v>54.2</v>
       </c>
-      <c r="J33" s="1" t="n">
+      <c r="K33" s="1" t="n">
         <v>1334.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>